<commit_message>
adding my php changes
</commit_message>
<xml_diff>
--- a/database_scripts/adhoc.xlsx
+++ b/database_scripts/adhoc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CoursePitt\Database\db_final_proj\database_scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A70E02-E5A5-446A-A139-99D26CE5E5BF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C96A87-6730-43DF-9B3E-B45F0DC913FF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4410" tabRatio="810" activeTab="10" xr2:uid="{748AF539-ECBA-4BE2-B14E-500CCCBD1977}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4410" tabRatio="810" activeTab="11" xr2:uid="{748AF539-ECBA-4BE2-B14E-500CCCBD1977}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="Sheet8" sheetId="8" r:id="rId9"/>
     <sheet name="Sheet7" sheetId="7" r:id="rId10"/>
     <sheet name="Sheet5" sheetId="11" r:id="rId11"/>
+    <sheet name="Sheet9" sheetId="12" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">insertMatchdetail2!$A$1:$J$67</definedName>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2447" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2476" uniqueCount="627">
   <si>
     <t>in  team1_id int,</t>
   </si>
@@ -1879,13 +1880,61 @@
   </si>
   <si>
     <t>);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$m_id </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $row["match_id"];</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$t1_id </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $row["team_id_1_fk"];</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$t2_id </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $row["team_id_2_fk"];</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$score_t1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $row['score_team_1'];</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$score_t2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $row['score_team_2'];</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$wicket_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $row['wicket_team_1'];</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$wicket_2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $row['wicket_team_2'];</t>
+  </si>
+  <si>
+    <t xml:space="preserve">echo </t>
+  </si>
+  <si>
+    <t>;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1893,13 +1942,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF660000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1914,9 +1975,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4385,7 +4452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D5F0DB7-BAAA-4FA2-B31A-11B1C7571D63}">
   <dimension ref="A2:C111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:C111"/>
     </sheetView>
   </sheetViews>
@@ -4411,7 +4478,7 @@
       </c>
       <c r="B3">
         <f ca="1">RANDBETWEEN(0,150)</f>
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
@@ -4423,7 +4490,7 @@
       </c>
       <c r="B4">
         <f ca="1">RANDBETWEEN(0,10)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>28</v>
@@ -4435,7 +4502,7 @@
       </c>
       <c r="B5">
         <f ca="1">RANDBETWEEN(0,60)</f>
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
         <v>28</v>
@@ -4447,7 +4514,7 @@
       </c>
       <c r="B6">
         <f ca="1">RANDBETWEEN(0,300)</f>
-        <v>204</v>
+        <v>69</v>
       </c>
       <c r="C6" t="s">
         <v>28</v>
@@ -4469,8 +4536,8 @@
         <v>183</v>
       </c>
       <c r="B8">
-        <f t="shared" ref="B8:B39" ca="1" si="0">RANDBETWEEN(0,150)</f>
-        <v>118</v>
+        <f t="shared" ref="B8" ca="1" si="0">RANDBETWEEN(0,150)</f>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
         <v>28</v>
@@ -4481,8 +4548,8 @@
         <v>184</v>
       </c>
       <c r="B9">
-        <f t="shared" ref="B9:B40" ca="1" si="1">RANDBETWEEN(0,10)</f>
-        <v>1</v>
+        <f t="shared" ref="B9" ca="1" si="1">RANDBETWEEN(0,10)</f>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
         <v>28</v>
@@ -4493,8 +4560,8 @@
         <v>185</v>
       </c>
       <c r="B10">
-        <f t="shared" ref="B10:B41" ca="1" si="2">RANDBETWEEN(0,60)</f>
-        <v>39</v>
+        <f t="shared" ref="B10" ca="1" si="2">RANDBETWEEN(0,60)</f>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
         <v>28</v>
@@ -4505,8 +4572,8 @@
         <v>186</v>
       </c>
       <c r="B11">
-        <f t="shared" ref="B11:B42" ca="1" si="3">RANDBETWEEN(0,300)</f>
-        <v>91</v>
+        <f t="shared" ref="B11" ca="1" si="3">RANDBETWEEN(0,300)</f>
+        <v>111</v>
       </c>
       <c r="C11" t="s">
         <v>28</v>
@@ -4528,8 +4595,8 @@
         <v>188</v>
       </c>
       <c r="B13">
-        <f t="shared" ref="B13:B44" ca="1" si="4">RANDBETWEEN(0,150)</f>
-        <v>72</v>
+        <f t="shared" ref="B13" ca="1" si="4">RANDBETWEEN(0,150)</f>
+        <v>69</v>
       </c>
       <c r="C13" t="s">
         <v>28</v>
@@ -4540,7 +4607,7 @@
         <v>189</v>
       </c>
       <c r="B14">
-        <f t="shared" ref="B14:B45" ca="1" si="5">RANDBETWEEN(0,10)</f>
+        <f t="shared" ref="B14" ca="1" si="5">RANDBETWEEN(0,10)</f>
         <v>5</v>
       </c>
       <c r="C14" t="s">
@@ -4552,8 +4619,8 @@
         <v>190</v>
       </c>
       <c r="B15">
-        <f t="shared" ref="B15:B46" ca="1" si="6">RANDBETWEEN(0,60)</f>
-        <v>35</v>
+        <f t="shared" ref="B15" ca="1" si="6">RANDBETWEEN(0,60)</f>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
         <v>28</v>
@@ -4564,8 +4631,8 @@
         <v>191</v>
       </c>
       <c r="B16">
-        <f t="shared" ref="B16:B47" ca="1" si="7">RANDBETWEEN(0,300)</f>
-        <v>13</v>
+        <f t="shared" ref="B16" ca="1" si="7">RANDBETWEEN(0,300)</f>
+        <v>148</v>
       </c>
       <c r="C16" t="s">
         <v>28</v>
@@ -4587,8 +4654,8 @@
         <v>193</v>
       </c>
       <c r="B18">
-        <f t="shared" ref="B18:B49" ca="1" si="8">RANDBETWEEN(0,150)</f>
-        <v>92</v>
+        <f t="shared" ref="B18" ca="1" si="8">RANDBETWEEN(0,150)</f>
+        <v>145</v>
       </c>
       <c r="C18" t="s">
         <v>28</v>
@@ -4599,8 +4666,8 @@
         <v>194</v>
       </c>
       <c r="B19">
-        <f t="shared" ref="B19:B50" ca="1" si="9">RANDBETWEEN(0,10)</f>
-        <v>3</v>
+        <f t="shared" ref="B19" ca="1" si="9">RANDBETWEEN(0,10)</f>
+        <v>2</v>
       </c>
       <c r="C19" t="s">
         <v>28</v>
@@ -4611,8 +4678,8 @@
         <v>195</v>
       </c>
       <c r="B20">
-        <f t="shared" ref="B20:B51" ca="1" si="10">RANDBETWEEN(0,60)</f>
-        <v>18</v>
+        <f t="shared" ref="B20" ca="1" si="10">RANDBETWEEN(0,60)</f>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>
@@ -4623,8 +4690,8 @@
         <v>196</v>
       </c>
       <c r="B21">
-        <f t="shared" ref="B21:B52" ca="1" si="11">RANDBETWEEN(0,300)</f>
-        <v>221</v>
+        <f t="shared" ref="B21" ca="1" si="11">RANDBETWEEN(0,300)</f>
+        <v>296</v>
       </c>
       <c r="C21" t="s">
         <v>28</v>
@@ -4646,8 +4713,8 @@
         <v>198</v>
       </c>
       <c r="B23">
-        <f t="shared" ref="B23:B54" ca="1" si="12">RANDBETWEEN(0,150)</f>
-        <v>86</v>
+        <f t="shared" ref="B23" ca="1" si="12">RANDBETWEEN(0,150)</f>
+        <v>66</v>
       </c>
       <c r="C23" t="s">
         <v>28</v>
@@ -4658,8 +4725,8 @@
         <v>199</v>
       </c>
       <c r="B24">
-        <f t="shared" ref="B24:B55" ca="1" si="13">RANDBETWEEN(0,10)</f>
-        <v>4</v>
+        <f t="shared" ref="B24" ca="1" si="13">RANDBETWEEN(0,10)</f>
+        <v>3</v>
       </c>
       <c r="C24" t="s">
         <v>28</v>
@@ -4670,8 +4737,8 @@
         <v>200</v>
       </c>
       <c r="B25">
-        <f t="shared" ref="B25:B56" ca="1" si="14">RANDBETWEEN(0,60)</f>
-        <v>36</v>
+        <f t="shared" ref="B25" ca="1" si="14">RANDBETWEEN(0,60)</f>
+        <v>16</v>
       </c>
       <c r="C25" t="s">
         <v>28</v>
@@ -4682,8 +4749,8 @@
         <v>201</v>
       </c>
       <c r="B26">
-        <f t="shared" ref="B26:B57" ca="1" si="15">RANDBETWEEN(0,300)</f>
-        <v>215</v>
+        <f t="shared" ref="B26" ca="1" si="15">RANDBETWEEN(0,300)</f>
+        <v>294</v>
       </c>
       <c r="C26" t="s">
         <v>28</v>
@@ -4705,8 +4772,8 @@
         <v>203</v>
       </c>
       <c r="B28">
-        <f t="shared" ref="B28:B59" ca="1" si="16">RANDBETWEEN(0,150)</f>
-        <v>13</v>
+        <f t="shared" ref="B28" ca="1" si="16">RANDBETWEEN(0,150)</f>
+        <v>59</v>
       </c>
       <c r="C28" t="s">
         <v>28</v>
@@ -4717,8 +4784,8 @@
         <v>204</v>
       </c>
       <c r="B29">
-        <f t="shared" ref="B29:B60" ca="1" si="17">RANDBETWEEN(0,10)</f>
-        <v>10</v>
+        <f t="shared" ref="B29" ca="1" si="17">RANDBETWEEN(0,10)</f>
+        <v>2</v>
       </c>
       <c r="C29" t="s">
         <v>28</v>
@@ -4729,8 +4796,8 @@
         <v>205</v>
       </c>
       <c r="B30">
-        <f t="shared" ref="B30:B61" ca="1" si="18">RANDBETWEEN(0,60)</f>
-        <v>13</v>
+        <f t="shared" ref="B30" ca="1" si="18">RANDBETWEEN(0,60)</f>
+        <v>17</v>
       </c>
       <c r="C30" t="s">
         <v>28</v>
@@ -4741,8 +4808,8 @@
         <v>206</v>
       </c>
       <c r="B31">
-        <f t="shared" ref="B31:B62" ca="1" si="19">RANDBETWEEN(0,300)</f>
-        <v>247</v>
+        <f t="shared" ref="B31" ca="1" si="19">RANDBETWEEN(0,300)</f>
+        <v>216</v>
       </c>
       <c r="C31" t="s">
         <v>28</v>
@@ -4764,8 +4831,8 @@
         <v>208</v>
       </c>
       <c r="B33">
-        <f t="shared" ref="B33:B64" ca="1" si="20">RANDBETWEEN(0,150)</f>
-        <v>60</v>
+        <f t="shared" ref="B33" ca="1" si="20">RANDBETWEEN(0,150)</f>
+        <v>53</v>
       </c>
       <c r="C33" t="s">
         <v>28</v>
@@ -4776,8 +4843,8 @@
         <v>209</v>
       </c>
       <c r="B34">
-        <f t="shared" ref="B34:B65" ca="1" si="21">RANDBETWEEN(0,10)</f>
-        <v>9</v>
+        <f t="shared" ref="B34" ca="1" si="21">RANDBETWEEN(0,10)</f>
+        <v>1</v>
       </c>
       <c r="C34" t="s">
         <v>28</v>
@@ -4788,8 +4855,8 @@
         <v>210</v>
       </c>
       <c r="B35">
-        <f t="shared" ref="B35:B66" ca="1" si="22">RANDBETWEEN(0,60)</f>
-        <v>40</v>
+        <f t="shared" ref="B35" ca="1" si="22">RANDBETWEEN(0,60)</f>
+        <v>50</v>
       </c>
       <c r="C35" t="s">
         <v>28</v>
@@ -4800,8 +4867,8 @@
         <v>211</v>
       </c>
       <c r="B36">
-        <f t="shared" ref="B36:B67" ca="1" si="23">RANDBETWEEN(0,300)</f>
-        <v>222</v>
+        <f t="shared" ref="B36" ca="1" si="23">RANDBETWEEN(0,300)</f>
+        <v>214</v>
       </c>
       <c r="C36" t="s">
         <v>28</v>
@@ -4823,8 +4890,8 @@
         <v>213</v>
       </c>
       <c r="B38">
-        <f t="shared" ref="B38:B69" ca="1" si="24">RANDBETWEEN(0,150)</f>
-        <v>124</v>
+        <f t="shared" ref="B38" ca="1" si="24">RANDBETWEEN(0,150)</f>
+        <v>110</v>
       </c>
       <c r="C38" t="s">
         <v>28</v>
@@ -4835,8 +4902,8 @@
         <v>214</v>
       </c>
       <c r="B39">
-        <f t="shared" ref="B39:B70" ca="1" si="25">RANDBETWEEN(0,10)</f>
-        <v>4</v>
+        <f t="shared" ref="B39" ca="1" si="25">RANDBETWEEN(0,10)</f>
+        <v>0</v>
       </c>
       <c r="C39" t="s">
         <v>28</v>
@@ -4847,8 +4914,8 @@
         <v>215</v>
       </c>
       <c r="B40">
-        <f t="shared" ref="B40:B71" ca="1" si="26">RANDBETWEEN(0,60)</f>
-        <v>32</v>
+        <f t="shared" ref="B40" ca="1" si="26">RANDBETWEEN(0,60)</f>
+        <v>19</v>
       </c>
       <c r="C40" t="s">
         <v>28</v>
@@ -4859,8 +4926,8 @@
         <v>216</v>
       </c>
       <c r="B41">
-        <f t="shared" ref="B41:B72" ca="1" si="27">RANDBETWEEN(0,300)</f>
-        <v>90</v>
+        <f t="shared" ref="B41" ca="1" si="27">RANDBETWEEN(0,300)</f>
+        <v>168</v>
       </c>
       <c r="C41" t="s">
         <v>28</v>
@@ -4882,8 +4949,8 @@
         <v>218</v>
       </c>
       <c r="B43">
-        <f t="shared" ref="B43:B74" ca="1" si="28">RANDBETWEEN(0,150)</f>
-        <v>59</v>
+        <f t="shared" ref="B43" ca="1" si="28">RANDBETWEEN(0,150)</f>
+        <v>41</v>
       </c>
       <c r="C43" t="s">
         <v>28</v>
@@ -4894,8 +4961,8 @@
         <v>219</v>
       </c>
       <c r="B44">
-        <f t="shared" ref="B44:B75" ca="1" si="29">RANDBETWEEN(0,10)</f>
-        <v>4</v>
+        <f t="shared" ref="B44" ca="1" si="29">RANDBETWEEN(0,10)</f>
+        <v>6</v>
       </c>
       <c r="C44" t="s">
         <v>28</v>
@@ -4906,8 +4973,8 @@
         <v>220</v>
       </c>
       <c r="B45">
-        <f t="shared" ref="B45:B76" ca="1" si="30">RANDBETWEEN(0,60)</f>
-        <v>55</v>
+        <f t="shared" ref="B45" ca="1" si="30">RANDBETWEEN(0,60)</f>
+        <v>32</v>
       </c>
       <c r="C45" t="s">
         <v>28</v>
@@ -4918,8 +4985,8 @@
         <v>221</v>
       </c>
       <c r="B46">
-        <f t="shared" ref="B46:B77" ca="1" si="31">RANDBETWEEN(0,300)</f>
-        <v>102</v>
+        <f t="shared" ref="B46" ca="1" si="31">RANDBETWEEN(0,300)</f>
+        <v>86</v>
       </c>
       <c r="C46" t="s">
         <v>28</v>
@@ -4941,8 +5008,8 @@
         <v>223</v>
       </c>
       <c r="B48">
-        <f t="shared" ref="B48:B79" ca="1" si="32">RANDBETWEEN(0,150)</f>
-        <v>85</v>
+        <f t="shared" ref="B48" ca="1" si="32">RANDBETWEEN(0,150)</f>
+        <v>51</v>
       </c>
       <c r="C48" t="s">
         <v>28</v>
@@ -4953,8 +5020,8 @@
         <v>224</v>
       </c>
       <c r="B49">
-        <f t="shared" ref="B49:B80" ca="1" si="33">RANDBETWEEN(0,10)</f>
-        <v>3</v>
+        <f t="shared" ref="B49" ca="1" si="33">RANDBETWEEN(0,10)</f>
+        <v>0</v>
       </c>
       <c r="C49" t="s">
         <v>28</v>
@@ -4965,8 +5032,8 @@
         <v>225</v>
       </c>
       <c r="B50">
-        <f t="shared" ref="B50:B81" ca="1" si="34">RANDBETWEEN(0,60)</f>
-        <v>59</v>
+        <f t="shared" ref="B50" ca="1" si="34">RANDBETWEEN(0,60)</f>
+        <v>47</v>
       </c>
       <c r="C50" t="s">
         <v>28</v>
@@ -4977,8 +5044,8 @@
         <v>226</v>
       </c>
       <c r="B51">
-        <f t="shared" ref="B51:B82" ca="1" si="35">RANDBETWEEN(0,300)</f>
-        <v>110</v>
+        <f t="shared" ref="B51" ca="1" si="35">RANDBETWEEN(0,300)</f>
+        <v>8</v>
       </c>
       <c r="C51" t="s">
         <v>28</v>
@@ -5000,8 +5067,8 @@
         <v>228</v>
       </c>
       <c r="B53">
-        <f t="shared" ref="B53:B84" ca="1" si="36">RANDBETWEEN(0,150)</f>
-        <v>142</v>
+        <f t="shared" ref="B53" ca="1" si="36">RANDBETWEEN(0,150)</f>
+        <v>103</v>
       </c>
       <c r="C53" t="s">
         <v>28</v>
@@ -5012,8 +5079,8 @@
         <v>229</v>
       </c>
       <c r="B54">
-        <f t="shared" ref="B54:B85" ca="1" si="37">RANDBETWEEN(0,10)</f>
-        <v>5</v>
+        <f t="shared" ref="B54" ca="1" si="37">RANDBETWEEN(0,10)</f>
+        <v>3</v>
       </c>
       <c r="C54" t="s">
         <v>28</v>
@@ -5024,8 +5091,8 @@
         <v>230</v>
       </c>
       <c r="B55">
-        <f t="shared" ref="B55:B86" ca="1" si="38">RANDBETWEEN(0,60)</f>
-        <v>28</v>
+        <f t="shared" ref="B55" ca="1" si="38">RANDBETWEEN(0,60)</f>
+        <v>19</v>
       </c>
       <c r="C55" t="s">
         <v>28</v>
@@ -5036,8 +5103,8 @@
         <v>231</v>
       </c>
       <c r="B56">
-        <f t="shared" ref="B56:B87" ca="1" si="39">RANDBETWEEN(0,300)</f>
-        <v>261</v>
+        <f t="shared" ref="B56" ca="1" si="39">RANDBETWEEN(0,300)</f>
+        <v>212</v>
       </c>
       <c r="C56" t="s">
         <v>28</v>
@@ -5059,8 +5126,8 @@
         <v>233</v>
       </c>
       <c r="B58">
-        <f t="shared" ref="B58:B89" ca="1" si="40">RANDBETWEEN(0,150)</f>
-        <v>96</v>
+        <f t="shared" ref="B58" ca="1" si="40">RANDBETWEEN(0,150)</f>
+        <v>112</v>
       </c>
       <c r="C58" t="s">
         <v>28</v>
@@ -5071,8 +5138,8 @@
         <v>234</v>
       </c>
       <c r="B59">
-        <f t="shared" ref="B59:B90" ca="1" si="41">RANDBETWEEN(0,10)</f>
-        <v>7</v>
+        <f t="shared" ref="B59" ca="1" si="41">RANDBETWEEN(0,10)</f>
+        <v>3</v>
       </c>
       <c r="C59" t="s">
         <v>28</v>
@@ -5083,8 +5150,8 @@
         <v>235</v>
       </c>
       <c r="B60">
-        <f t="shared" ref="B60:B91" ca="1" si="42">RANDBETWEEN(0,60)</f>
-        <v>3</v>
+        <f t="shared" ref="B60" ca="1" si="42">RANDBETWEEN(0,60)</f>
+        <v>15</v>
       </c>
       <c r="C60" t="s">
         <v>28</v>
@@ -5095,8 +5162,8 @@
         <v>236</v>
       </c>
       <c r="B61">
-        <f t="shared" ref="B61:B92" ca="1" si="43">RANDBETWEEN(0,300)</f>
-        <v>24</v>
+        <f t="shared" ref="B61" ca="1" si="43">RANDBETWEEN(0,300)</f>
+        <v>296</v>
       </c>
       <c r="C61" t="s">
         <v>28</v>
@@ -5118,8 +5185,8 @@
         <v>238</v>
       </c>
       <c r="B63">
-        <f t="shared" ref="B63:B94" ca="1" si="44">RANDBETWEEN(0,150)</f>
-        <v>21</v>
+        <f t="shared" ref="B63" ca="1" si="44">RANDBETWEEN(0,150)</f>
+        <v>81</v>
       </c>
       <c r="C63" t="s">
         <v>28</v>
@@ -5130,8 +5197,8 @@
         <v>239</v>
       </c>
       <c r="B64">
-        <f t="shared" ref="B64:B111" ca="1" si="45">RANDBETWEEN(0,10)</f>
-        <v>5</v>
+        <f t="shared" ref="B64" ca="1" si="45">RANDBETWEEN(0,10)</f>
+        <v>8</v>
       </c>
       <c r="C64" t="s">
         <v>28</v>
@@ -5142,8 +5209,8 @@
         <v>240</v>
       </c>
       <c r="B65">
-        <f t="shared" ref="B65:B111" ca="1" si="46">RANDBETWEEN(0,60)</f>
-        <v>8</v>
+        <f t="shared" ref="B65" ca="1" si="46">RANDBETWEEN(0,60)</f>
+        <v>52</v>
       </c>
       <c r="C65" t="s">
         <v>28</v>
@@ -5154,8 +5221,8 @@
         <v>241</v>
       </c>
       <c r="B66">
-        <f t="shared" ref="B66:B111" ca="1" si="47">RANDBETWEEN(0,300)</f>
-        <v>170</v>
+        <f t="shared" ref="B66" ca="1" si="47">RANDBETWEEN(0,300)</f>
+        <v>235</v>
       </c>
       <c r="C66" t="s">
         <v>28</v>
@@ -5177,8 +5244,8 @@
         <v>243</v>
       </c>
       <c r="B68">
-        <f t="shared" ref="B68:B111" ca="1" si="48">RANDBETWEEN(0,150)</f>
-        <v>131</v>
+        <f t="shared" ref="B68" ca="1" si="48">RANDBETWEEN(0,150)</f>
+        <v>109</v>
       </c>
       <c r="C68" t="s">
         <v>28</v>
@@ -5189,8 +5256,8 @@
         <v>244</v>
       </c>
       <c r="B69">
-        <f t="shared" ref="B69:B111" ca="1" si="49">RANDBETWEEN(0,10)</f>
-        <v>6</v>
+        <f t="shared" ref="B69" ca="1" si="49">RANDBETWEEN(0,10)</f>
+        <v>7</v>
       </c>
       <c r="C69" t="s">
         <v>28</v>
@@ -5201,8 +5268,8 @@
         <v>245</v>
       </c>
       <c r="B70">
-        <f t="shared" ref="B70:B111" ca="1" si="50">RANDBETWEEN(0,60)</f>
-        <v>36</v>
+        <f t="shared" ref="B70" ca="1" si="50">RANDBETWEEN(0,60)</f>
+        <v>9</v>
       </c>
       <c r="C70" t="s">
         <v>28</v>
@@ -5213,8 +5280,8 @@
         <v>246</v>
       </c>
       <c r="B71">
-        <f t="shared" ref="B71:B111" ca="1" si="51">RANDBETWEEN(0,300)</f>
-        <v>57</v>
+        <f t="shared" ref="B71" ca="1" si="51">RANDBETWEEN(0,300)</f>
+        <v>185</v>
       </c>
       <c r="C71" t="s">
         <v>28</v>
@@ -5236,8 +5303,8 @@
         <v>248</v>
       </c>
       <c r="B73">
-        <f t="shared" ref="B73:B111" ca="1" si="52">RANDBETWEEN(0,150)</f>
-        <v>59</v>
+        <f t="shared" ref="B73" ca="1" si="52">RANDBETWEEN(0,150)</f>
+        <v>95</v>
       </c>
       <c r="C73" t="s">
         <v>28</v>
@@ -5248,8 +5315,8 @@
         <v>249</v>
       </c>
       <c r="B74">
-        <f t="shared" ref="B74:B111" ca="1" si="53">RANDBETWEEN(0,10)</f>
-        <v>3</v>
+        <f t="shared" ref="B74" ca="1" si="53">RANDBETWEEN(0,10)</f>
+        <v>8</v>
       </c>
       <c r="C74" t="s">
         <v>28</v>
@@ -5260,8 +5327,8 @@
         <v>250</v>
       </c>
       <c r="B75">
-        <f t="shared" ref="B75:B111" ca="1" si="54">RANDBETWEEN(0,60)</f>
-        <v>22</v>
+        <f t="shared" ref="B75" ca="1" si="54">RANDBETWEEN(0,60)</f>
+        <v>37</v>
       </c>
       <c r="C75" t="s">
         <v>28</v>
@@ -5272,8 +5339,8 @@
         <v>251</v>
       </c>
       <c r="B76">
-        <f t="shared" ref="B76:B111" ca="1" si="55">RANDBETWEEN(0,300)</f>
-        <v>116</v>
+        <f t="shared" ref="B76" ca="1" si="55">RANDBETWEEN(0,300)</f>
+        <v>148</v>
       </c>
       <c r="C76" t="s">
         <v>28</v>
@@ -5295,8 +5362,8 @@
         <v>253</v>
       </c>
       <c r="B78">
-        <f t="shared" ref="B78:B111" ca="1" si="56">RANDBETWEEN(0,150)</f>
-        <v>51</v>
+        <f t="shared" ref="B78" ca="1" si="56">RANDBETWEEN(0,150)</f>
+        <v>110</v>
       </c>
       <c r="C78" t="s">
         <v>28</v>
@@ -5307,8 +5374,8 @@
         <v>254</v>
       </c>
       <c r="B79">
-        <f t="shared" ref="B79:B111" ca="1" si="57">RANDBETWEEN(0,10)</f>
-        <v>2</v>
+        <f t="shared" ref="B79" ca="1" si="57">RANDBETWEEN(0,10)</f>
+        <v>6</v>
       </c>
       <c r="C79" t="s">
         <v>28</v>
@@ -5319,8 +5386,8 @@
         <v>255</v>
       </c>
       <c r="B80">
-        <f t="shared" ref="B80:B111" ca="1" si="58">RANDBETWEEN(0,60)</f>
-        <v>12</v>
+        <f t="shared" ref="B80" ca="1" si="58">RANDBETWEEN(0,60)</f>
+        <v>39</v>
       </c>
       <c r="C80" t="s">
         <v>28</v>
@@ -5331,8 +5398,8 @@
         <v>256</v>
       </c>
       <c r="B81">
-        <f t="shared" ref="B81:B111" ca="1" si="59">RANDBETWEEN(0,300)</f>
-        <v>76</v>
+        <f t="shared" ref="B81" ca="1" si="59">RANDBETWEEN(0,300)</f>
+        <v>125</v>
       </c>
       <c r="C81" t="s">
         <v>28</v>
@@ -5354,8 +5421,8 @@
         <v>258</v>
       </c>
       <c r="B83">
-        <f t="shared" ref="B83:B111" ca="1" si="60">RANDBETWEEN(0,150)</f>
-        <v>35</v>
+        <f t="shared" ref="B83" ca="1" si="60">RANDBETWEEN(0,150)</f>
+        <v>112</v>
       </c>
       <c r="C83" t="s">
         <v>28</v>
@@ -5366,7 +5433,7 @@
         <v>259</v>
       </c>
       <c r="B84">
-        <f t="shared" ref="B84:B111" ca="1" si="61">RANDBETWEEN(0,10)</f>
+        <f t="shared" ref="B84" ca="1" si="61">RANDBETWEEN(0,10)</f>
         <v>6</v>
       </c>
       <c r="C84" t="s">
@@ -5378,8 +5445,8 @@
         <v>260</v>
       </c>
       <c r="B85">
-        <f t="shared" ref="B85:B111" ca="1" si="62">RANDBETWEEN(0,60)</f>
-        <v>42</v>
+        <f t="shared" ref="B85" ca="1" si="62">RANDBETWEEN(0,60)</f>
+        <v>17</v>
       </c>
       <c r="C85" t="s">
         <v>28</v>
@@ -5390,8 +5457,8 @@
         <v>261</v>
       </c>
       <c r="B86">
-        <f t="shared" ref="B86:B111" ca="1" si="63">RANDBETWEEN(0,300)</f>
-        <v>238</v>
+        <f t="shared" ref="B86" ca="1" si="63">RANDBETWEEN(0,300)</f>
+        <v>191</v>
       </c>
       <c r="C86" t="s">
         <v>28</v>
@@ -5413,8 +5480,8 @@
         <v>263</v>
       </c>
       <c r="B88">
-        <f t="shared" ref="B88:B111" ca="1" si="64">RANDBETWEEN(0,150)</f>
-        <v>30</v>
+        <f t="shared" ref="B88" ca="1" si="64">RANDBETWEEN(0,150)</f>
+        <v>60</v>
       </c>
       <c r="C88" t="s">
         <v>28</v>
@@ -5425,8 +5492,8 @@
         <v>264</v>
       </c>
       <c r="B89">
-        <f t="shared" ref="B89:B111" ca="1" si="65">RANDBETWEEN(0,10)</f>
-        <v>0</v>
+        <f t="shared" ref="B89" ca="1" si="65">RANDBETWEEN(0,10)</f>
+        <v>7</v>
       </c>
       <c r="C89" t="s">
         <v>28</v>
@@ -5437,8 +5504,8 @@
         <v>265</v>
       </c>
       <c r="B90">
-        <f t="shared" ref="B90:B111" ca="1" si="66">RANDBETWEEN(0,60)</f>
-        <v>21</v>
+        <f t="shared" ref="B90" ca="1" si="66">RANDBETWEEN(0,60)</f>
+        <v>11</v>
       </c>
       <c r="C90" t="s">
         <v>28</v>
@@ -5449,8 +5516,8 @@
         <v>266</v>
       </c>
       <c r="B91">
-        <f t="shared" ref="B91:B111" ca="1" si="67">RANDBETWEEN(0,300)</f>
-        <v>282</v>
+        <f t="shared" ref="B91" ca="1" si="67">RANDBETWEEN(0,300)</f>
+        <v>251</v>
       </c>
       <c r="C91" t="s">
         <v>28</v>
@@ -5472,8 +5539,8 @@
         <v>268</v>
       </c>
       <c r="B93">
-        <f t="shared" ref="B93:B111" ca="1" si="68">RANDBETWEEN(0,150)</f>
-        <v>42</v>
+        <f t="shared" ref="B93" ca="1" si="68">RANDBETWEEN(0,150)</f>
+        <v>57</v>
       </c>
       <c r="C93" t="s">
         <v>28</v>
@@ -5484,8 +5551,8 @@
         <v>269</v>
       </c>
       <c r="B94">
-        <f t="shared" ref="B94:B111" ca="1" si="69">RANDBETWEEN(0,10)</f>
-        <v>3</v>
+        <f t="shared" ref="B94" ca="1" si="69">RANDBETWEEN(0,10)</f>
+        <v>6</v>
       </c>
       <c r="C94" t="s">
         <v>28</v>
@@ -5496,8 +5563,8 @@
         <v>270</v>
       </c>
       <c r="B95">
-        <f t="shared" ref="B95:B111" ca="1" si="70">RANDBETWEEN(0,60)</f>
-        <v>20</v>
+        <f t="shared" ref="B95" ca="1" si="70">RANDBETWEEN(0,60)</f>
+        <v>26</v>
       </c>
       <c r="C95" t="s">
         <v>28</v>
@@ -5508,8 +5575,8 @@
         <v>271</v>
       </c>
       <c r="B96">
-        <f t="shared" ref="B96:B111" ca="1" si="71">RANDBETWEEN(0,300)</f>
-        <v>20</v>
+        <f t="shared" ref="B96" ca="1" si="71">RANDBETWEEN(0,300)</f>
+        <v>198</v>
       </c>
       <c r="C96" t="s">
         <v>28</v>
@@ -5531,8 +5598,8 @@
         <v>273</v>
       </c>
       <c r="B98">
-        <f t="shared" ref="B98:B111" ca="1" si="72">RANDBETWEEN(0,150)</f>
-        <v>90</v>
+        <f t="shared" ref="B98" ca="1" si="72">RANDBETWEEN(0,150)</f>
+        <v>16</v>
       </c>
       <c r="C98" t="s">
         <v>28</v>
@@ -5543,8 +5610,8 @@
         <v>274</v>
       </c>
       <c r="B99">
-        <f t="shared" ref="B99:B111" ca="1" si="73">RANDBETWEEN(0,10)</f>
-        <v>3</v>
+        <f t="shared" ref="B99" ca="1" si="73">RANDBETWEEN(0,10)</f>
+        <v>5</v>
       </c>
       <c r="C99" t="s">
         <v>28</v>
@@ -5555,8 +5622,8 @@
         <v>275</v>
       </c>
       <c r="B100">
-        <f t="shared" ref="B100:B111" ca="1" si="74">RANDBETWEEN(0,60)</f>
-        <v>59</v>
+        <f t="shared" ref="B100" ca="1" si="74">RANDBETWEEN(0,60)</f>
+        <v>39</v>
       </c>
       <c r="C100" t="s">
         <v>28</v>
@@ -5567,8 +5634,8 @@
         <v>276</v>
       </c>
       <c r="B101">
-        <f t="shared" ref="B101:B111" ca="1" si="75">RANDBETWEEN(0,300)</f>
-        <v>61</v>
+        <f t="shared" ref="B101" ca="1" si="75">RANDBETWEEN(0,300)</f>
+        <v>47</v>
       </c>
       <c r="C101" t="s">
         <v>28</v>
@@ -5590,8 +5657,8 @@
         <v>278</v>
       </c>
       <c r="B103">
-        <f t="shared" ref="B103:B111" ca="1" si="76">RANDBETWEEN(0,150)</f>
-        <v>31</v>
+        <f t="shared" ref="B103" ca="1" si="76">RANDBETWEEN(0,150)</f>
+        <v>37</v>
       </c>
       <c r="C103" t="s">
         <v>28</v>
@@ -5602,8 +5669,8 @@
         <v>279</v>
       </c>
       <c r="B104">
-        <f t="shared" ref="B104:B111" ca="1" si="77">RANDBETWEEN(0,10)</f>
-        <v>1</v>
+        <f t="shared" ref="B104" ca="1" si="77">RANDBETWEEN(0,10)</f>
+        <v>5</v>
       </c>
       <c r="C104" t="s">
         <v>28</v>
@@ -5614,8 +5681,8 @@
         <v>280</v>
       </c>
       <c r="B105">
-        <f t="shared" ref="B105:B111" ca="1" si="78">RANDBETWEEN(0,60)</f>
-        <v>1</v>
+        <f t="shared" ref="B105" ca="1" si="78">RANDBETWEEN(0,60)</f>
+        <v>23</v>
       </c>
       <c r="C105" t="s">
         <v>28</v>
@@ -5626,8 +5693,8 @@
         <v>281</v>
       </c>
       <c r="B106">
-        <f t="shared" ref="B106:B111" ca="1" si="79">RANDBETWEEN(0,300)</f>
-        <v>19</v>
+        <f t="shared" ref="B106" ca="1" si="79">RANDBETWEEN(0,300)</f>
+        <v>181</v>
       </c>
       <c r="C106" t="s">
         <v>28</v>
@@ -5649,8 +5716,8 @@
         <v>283</v>
       </c>
       <c r="B108">
-        <f t="shared" ref="B108:B111" ca="1" si="80">RANDBETWEEN(0,150)</f>
-        <v>29</v>
+        <f t="shared" ref="B108" ca="1" si="80">RANDBETWEEN(0,150)</f>
+        <v>99</v>
       </c>
       <c r="C108" t="s">
         <v>28</v>
@@ -5661,8 +5728,8 @@
         <v>284</v>
       </c>
       <c r="B109">
-        <f t="shared" ref="B109:B111" ca="1" si="81">RANDBETWEEN(0,10)</f>
-        <v>2</v>
+        <f t="shared" ref="B109" ca="1" si="81">RANDBETWEEN(0,10)</f>
+        <v>5</v>
       </c>
       <c r="C109" t="s">
         <v>28</v>
@@ -5673,8 +5740,8 @@
         <v>285</v>
       </c>
       <c r="B110">
-        <f t="shared" ref="B110:B111" ca="1" si="82">RANDBETWEEN(0,60)</f>
-        <v>23</v>
+        <f t="shared" ref="B110" ca="1" si="82">RANDBETWEEN(0,60)</f>
+        <v>9</v>
       </c>
       <c r="C110" t="s">
         <v>28</v>
@@ -5686,7 +5753,7 @@
       </c>
       <c r="B111">
         <f t="shared" ref="B111" ca="1" si="83">RANDBETWEEN(0,300)</f>
-        <v>191</v>
+        <v>55</v>
       </c>
       <c r="C111" t="s">
         <v>28</v>
@@ -5699,6 +5766,129 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AD0EE8C-2A75-4924-A9E5-A3E43A503A30}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>625</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="D1" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>625</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="D2" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>625</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>615</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="D3" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>625</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="D4" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>625</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="D5" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>625</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="D6" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>625</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="D7" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>